<commit_message>
Matrix Algorithms organized as per logic pattern
</commit_message>
<xml_diff>
--- a/0.0 - Common/NeedfulAnalysisInfo.xlsx
+++ b/0.0 - Common/NeedfulAnalysisInfo.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SrigopalSAI\VSOnlineDemo\DataStructures And Algorithms\0.0 - Common\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SaiSMAPersonal\SaiSRIWork\Education\DSndAlgos\0.0 - Common\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="6120" tabRatio="831" firstSheet="1" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="6120" tabRatio="831" firstSheet="1" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Complexity" sheetId="5" r:id="rId1"/>
@@ -27,7 +27,7 @@
     <sheet name="List" sheetId="21" r:id="rId13"/>
     <sheet name="Testing" sheetId="12" r:id="rId14"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -7482,7 +7482,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="35">
     <font>
       <sz val="11"/>
@@ -8788,14 +8788,56 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -8805,12 +8847,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
@@ -8820,66 +8856,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -8893,18 +8905,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -8956,11 +8956,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -11036,7 +11036,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H85"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -11411,219 +11411,219 @@
       <c r="A25" s="183"/>
     </row>
     <row r="26" spans="1:6" ht="59.25" customHeight="1">
-      <c r="A26" s="221" t="s">
+      <c r="A26" s="236" t="s">
         <v>63</v>
       </c>
-      <c r="B26" s="221"/>
-      <c r="C26" s="221"/>
-      <c r="D26" s="221"/>
-      <c r="E26" s="221"/>
+      <c r="B26" s="236"/>
+      <c r="C26" s="236"/>
+      <c r="D26" s="236"/>
+      <c r="E26" s="236"/>
     </row>
     <row r="27" spans="1:6" ht="33.75" customHeight="1">
       <c r="A27" s="183"/>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="222" t="s">
+      <c r="A28" s="237" t="s">
         <v>64</v>
       </c>
-      <c r="B28" s="223"/>
-      <c r="C28" s="223"/>
-      <c r="D28" s="223"/>
-      <c r="E28" s="223"/>
-      <c r="F28" s="224"/>
+      <c r="B28" s="235"/>
+      <c r="C28" s="235"/>
+      <c r="D28" s="235"/>
+      <c r="E28" s="235"/>
+      <c r="F28" s="238"/>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="222" t="s">
+      <c r="A29" s="237" t="s">
         <v>65</v>
       </c>
-      <c r="B29" s="223"/>
-      <c r="C29" s="223"/>
-      <c r="D29" s="223"/>
-      <c r="E29" s="223"/>
-      <c r="F29" s="224"/>
+      <c r="B29" s="235"/>
+      <c r="C29" s="235"/>
+      <c r="D29" s="235"/>
+      <c r="E29" s="235"/>
+      <c r="F29" s="238"/>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="225" t="s">
+      <c r="A30" s="239" t="s">
         <v>66</v>
       </c>
-      <c r="B30" s="223"/>
-      <c r="C30" s="223"/>
-      <c r="D30" s="223"/>
-      <c r="E30" s="223"/>
-      <c r="F30" s="224"/>
+      <c r="B30" s="235"/>
+      <c r="C30" s="235"/>
+      <c r="D30" s="235"/>
+      <c r="E30" s="235"/>
+      <c r="F30" s="238"/>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="231" t="s">
+      <c r="A31" s="243" t="s">
         <v>67</v>
       </c>
-      <c r="B31" s="231"/>
-      <c r="C31" s="231"/>
-      <c r="D31" s="231"/>
-      <c r="E31" s="231"/>
+      <c r="B31" s="243"/>
+      <c r="C31" s="243"/>
+      <c r="D31" s="243"/>
+      <c r="E31" s="243"/>
       <c r="F31" s="199"/>
     </row>
     <row r="32" spans="1:6" ht="33" customHeight="1">
-      <c r="A32" s="233" t="s">
+      <c r="A32" s="226" t="s">
         <v>68</v>
       </c>
-      <c r="B32" s="234"/>
-      <c r="C32" s="234"/>
-      <c r="D32" s="234"/>
-      <c r="E32" s="234"/>
-      <c r="F32" s="235"/>
+      <c r="B32" s="227"/>
+      <c r="C32" s="227"/>
+      <c r="D32" s="227"/>
+      <c r="E32" s="227"/>
+      <c r="F32" s="228"/>
     </row>
     <row r="33" spans="1:7" ht="93.75" customHeight="1">
-      <c r="A33" s="236" t="s">
+      <c r="A33" s="229" t="s">
         <v>69</v>
       </c>
-      <c r="B33" s="237"/>
-      <c r="C33" s="237"/>
-      <c r="D33" s="237"/>
-      <c r="E33" s="237"/>
-      <c r="F33" s="237"/>
+      <c r="B33" s="230"/>
+      <c r="C33" s="230"/>
+      <c r="D33" s="230"/>
+      <c r="E33" s="230"/>
+      <c r="F33" s="230"/>
     </row>
     <row r="34" spans="1:7" ht="42" customHeight="1">
-      <c r="A34" s="226" t="s">
+      <c r="A34" s="240" t="s">
         <v>70</v>
       </c>
-      <c r="B34" s="227"/>
-      <c r="C34" s="227"/>
-      <c r="D34" s="227"/>
-      <c r="E34" s="227"/>
-      <c r="F34" s="227"/>
+      <c r="B34" s="225"/>
+      <c r="C34" s="225"/>
+      <c r="D34" s="225"/>
+      <c r="E34" s="225"/>
+      <c r="F34" s="225"/>
     </row>
     <row r="35" spans="1:7" ht="69" customHeight="1">
-      <c r="A35" s="227" t="s">
+      <c r="A35" s="225" t="s">
         <v>71</v>
       </c>
-      <c r="B35" s="227"/>
-      <c r="C35" s="227"/>
-      <c r="D35" s="227"/>
-      <c r="E35" s="227"/>
-      <c r="F35" s="227"/>
+      <c r="B35" s="225"/>
+      <c r="C35" s="225"/>
+      <c r="D35" s="225"/>
+      <c r="E35" s="225"/>
+      <c r="F35" s="225"/>
     </row>
     <row r="36" spans="1:7" ht="87.75" customHeight="1">
-      <c r="A36" s="229" t="s">
+      <c r="A36" s="241" t="s">
         <v>72</v>
       </c>
-      <c r="B36" s="229"/>
-      <c r="C36" s="229"/>
-      <c r="D36" s="229"/>
+      <c r="B36" s="241"/>
+      <c r="C36" s="241"/>
+      <c r="D36" s="241"/>
     </row>
     <row r="37" spans="1:7" ht="105" customHeight="1">
-      <c r="A37" s="230" t="s">
+      <c r="A37" s="242" t="s">
         <v>73</v>
       </c>
-      <c r="B37" s="230"/>
-      <c r="C37" s="230"/>
-      <c r="D37" s="230"/>
-      <c r="E37" s="230"/>
+      <c r="B37" s="242"/>
+      <c r="C37" s="242"/>
+      <c r="D37" s="242"/>
+      <c r="E37" s="242"/>
     </row>
     <row r="38" spans="1:7" ht="152.25" customHeight="1">
-      <c r="A38" s="223" t="s">
+      <c r="A38" s="235" t="s">
         <v>74</v>
       </c>
-      <c r="B38" s="223"/>
-      <c r="C38" s="223"/>
-      <c r="D38" s="223"/>
+      <c r="B38" s="235"/>
+      <c r="C38" s="235"/>
+      <c r="D38" s="235"/>
       <c r="E38" s="187"/>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="232" t="s">
+      <c r="A39" s="233" t="s">
         <v>75</v>
       </c>
-      <c r="B39" s="232"/>
-      <c r="C39" s="232"/>
+      <c r="B39" s="233"/>
+      <c r="C39" s="233"/>
       <c r="D39" s="74" t="s">
         <v>76</v>
       </c>
-      <c r="E39" s="240" t="s">
+      <c r="E39" s="232" t="s">
         <v>77</v>
       </c>
-      <c r="F39" s="232"/>
-      <c r="G39" s="232"/>
+      <c r="F39" s="233"/>
+      <c r="G39" s="233"/>
     </row>
     <row r="40" spans="1:7" ht="145.5" customHeight="1">
-      <c r="A40" s="228" t="s">
+      <c r="A40" s="231" t="s">
         <v>78</v>
       </c>
-      <c r="B40" s="228"/>
-      <c r="C40" s="228"/>
-      <c r="D40" s="228"/>
-      <c r="E40" s="228"/>
-      <c r="F40" s="228"/>
+      <c r="B40" s="231"/>
+      <c r="C40" s="231"/>
+      <c r="D40" s="231"/>
+      <c r="E40" s="231"/>
+      <c r="F40" s="231"/>
       <c r="G40" s="199"/>
     </row>
     <row r="41" spans="1:7" ht="57.75" customHeight="1">
-      <c r="A41" s="228" t="s">
+      <c r="A41" s="231" t="s">
         <v>79</v>
       </c>
-      <c r="B41" s="228"/>
-      <c r="C41" s="228"/>
-      <c r="D41" s="228"/>
-      <c r="E41" s="228"/>
-      <c r="F41" s="228"/>
+      <c r="B41" s="231"/>
+      <c r="C41" s="231"/>
+      <c r="D41" s="231"/>
+      <c r="E41" s="231"/>
+      <c r="F41" s="231"/>
       <c r="G41" s="199"/>
     </row>
     <row r="42" spans="1:7" ht="118.5" customHeight="1">
-      <c r="A42" s="228" t="s">
+      <c r="A42" s="231" t="s">
         <v>80</v>
       </c>
-      <c r="B42" s="228"/>
-      <c r="C42" s="228"/>
-      <c r="D42" s="228"/>
-      <c r="E42" s="228"/>
-      <c r="F42" s="228"/>
+      <c r="B42" s="231"/>
+      <c r="C42" s="231"/>
+      <c r="D42" s="231"/>
+      <c r="E42" s="231"/>
+      <c r="F42" s="231"/>
       <c r="G42" s="199"/>
     </row>
     <row r="43" spans="1:7" ht="32.25" customHeight="1">
-      <c r="A43" s="228" t="s">
+      <c r="A43" s="231" t="s">
         <v>81</v>
       </c>
-      <c r="B43" s="228"/>
-      <c r="C43" s="228"/>
-      <c r="D43" s="228"/>
-      <c r="E43" s="228"/>
-      <c r="F43" s="228"/>
+      <c r="B43" s="231"/>
+      <c r="C43" s="231"/>
+      <c r="D43" s="231"/>
+      <c r="E43" s="231"/>
+      <c r="F43" s="231"/>
       <c r="G43" s="199"/>
     </row>
     <row r="44" spans="1:7" ht="120.75" customHeight="1">
-      <c r="A44" s="228" t="s">
+      <c r="A44" s="231" t="s">
         <v>82</v>
       </c>
-      <c r="B44" s="228"/>
-      <c r="C44" s="228"/>
-      <c r="D44" s="228"/>
-      <c r="E44" s="228"/>
-      <c r="F44" s="228"/>
+      <c r="B44" s="231"/>
+      <c r="C44" s="231"/>
+      <c r="D44" s="231"/>
+      <c r="E44" s="231"/>
+      <c r="F44" s="231"/>
       <c r="G44" s="199"/>
     </row>
     <row r="45" spans="1:7">
-      <c r="A45" s="228" t="s">
+      <c r="A45" s="231" t="s">
         <v>83</v>
       </c>
-      <c r="B45" s="228"/>
-      <c r="C45" s="228"/>
-      <c r="D45" s="228"/>
-      <c r="E45" s="228"/>
-      <c r="F45" s="228"/>
+      <c r="B45" s="231"/>
+      <c r="C45" s="231"/>
+      <c r="D45" s="231"/>
+      <c r="E45" s="231"/>
+      <c r="F45" s="231"/>
       <c r="G45" s="199"/>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="239"/>
-      <c r="B46" s="239"/>
-      <c r="C46" s="239"/>
-      <c r="D46" s="239"/>
-      <c r="E46" s="239"/>
-      <c r="F46" s="239"/>
+      <c r="A46" s="222"/>
+      <c r="B46" s="222"/>
+      <c r="C46" s="222"/>
+      <c r="D46" s="222"/>
+      <c r="E46" s="222"/>
+      <c r="F46" s="222"/>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="239"/>
-      <c r="B47" s="239"/>
-      <c r="C47" s="239"/>
-      <c r="D47" s="239"/>
-      <c r="E47" s="239"/>
-      <c r="F47" s="239"/>
+      <c r="A47" s="222"/>
+      <c r="B47" s="222"/>
+      <c r="C47" s="222"/>
+      <c r="D47" s="222"/>
+      <c r="E47" s="222"/>
+      <c r="F47" s="222"/>
     </row>
     <row r="49" spans="1:8" ht="16.5">
       <c r="A49" s="183"/>
@@ -11676,174 +11676,174 @@
       <c r="E54" s="199"/>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="242" t="s">
+      <c r="A57" s="224" t="s">
         <v>94</v>
       </c>
-      <c r="B57" s="242"/>
-      <c r="C57" s="242"/>
+      <c r="B57" s="224"/>
+      <c r="C57" s="224"/>
     </row>
     <row r="58" spans="1:8" ht="140.25" customHeight="1">
-      <c r="A58" s="241" t="s">
+      <c r="A58" s="234" t="s">
         <v>95</v>
       </c>
-      <c r="B58" s="241"/>
-      <c r="C58" s="241"/>
-      <c r="D58" s="241"/>
-      <c r="E58" s="241"/>
-      <c r="F58" s="241"/>
-      <c r="G58" s="241"/>
+      <c r="B58" s="234"/>
+      <c r="C58" s="234"/>
+      <c r="D58" s="234"/>
+      <c r="E58" s="234"/>
+      <c r="F58" s="234"/>
+      <c r="G58" s="234"/>
       <c r="H58" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="59" spans="1:8">
-      <c r="A59" s="239" t="s">
+      <c r="A59" s="222" t="s">
         <v>97</v>
       </c>
-      <c r="B59" s="239"/>
-      <c r="C59" s="239"/>
-      <c r="D59" s="239"/>
-      <c r="E59" s="239"/>
-      <c r="F59" s="239"/>
+      <c r="B59" s="222"/>
+      <c r="C59" s="222"/>
+      <c r="D59" s="222"/>
+      <c r="E59" s="222"/>
+      <c r="F59" s="222"/>
     </row>
     <row r="60" spans="1:8">
-      <c r="A60" s="238" t="s">
+      <c r="A60" s="223" t="s">
         <v>98</v>
       </c>
-      <c r="B60" s="239"/>
-      <c r="C60" s="239"/>
-      <c r="D60" s="239"/>
-      <c r="E60" s="239"/>
-      <c r="F60" s="239"/>
+      <c r="B60" s="222"/>
+      <c r="C60" s="222"/>
+      <c r="D60" s="222"/>
+      <c r="E60" s="222"/>
+      <c r="F60" s="222"/>
     </row>
     <row r="61" spans="1:8">
-      <c r="A61" s="238" t="s">
+      <c r="A61" s="223" t="s">
         <v>99</v>
       </c>
-      <c r="B61" s="239"/>
-      <c r="C61" s="239"/>
-      <c r="D61" s="239"/>
-      <c r="E61" s="239"/>
-      <c r="F61" s="239"/>
+      <c r="B61" s="222"/>
+      <c r="C61" s="222"/>
+      <c r="D61" s="222"/>
+      <c r="E61" s="222"/>
+      <c r="F61" s="222"/>
     </row>
     <row r="62" spans="1:8">
-      <c r="A62" s="238" t="s">
+      <c r="A62" s="223" t="s">
         <v>100</v>
       </c>
-      <c r="B62" s="239"/>
-      <c r="C62" s="239"/>
-      <c r="D62" s="239"/>
-      <c r="E62" s="239"/>
-      <c r="F62" s="239"/>
+      <c r="B62" s="222"/>
+      <c r="C62" s="222"/>
+      <c r="D62" s="222"/>
+      <c r="E62" s="222"/>
+      <c r="F62" s="222"/>
     </row>
     <row r="63" spans="1:8">
-      <c r="A63" s="238" t="s">
+      <c r="A63" s="223" t="s">
         <v>101</v>
       </c>
-      <c r="B63" s="239"/>
-      <c r="C63" s="239"/>
-      <c r="D63" s="239"/>
-      <c r="E63" s="239"/>
-      <c r="F63" s="239"/>
+      <c r="B63" s="222"/>
+      <c r="C63" s="222"/>
+      <c r="D63" s="222"/>
+      <c r="E63" s="222"/>
+      <c r="F63" s="222"/>
     </row>
     <row r="64" spans="1:8">
-      <c r="A64" s="242" t="s">
+      <c r="A64" s="224" t="s">
         <v>102</v>
       </c>
-      <c r="B64" s="242"/>
-      <c r="C64" s="242"/>
+      <c r="B64" s="224"/>
+      <c r="C64" s="224"/>
     </row>
     <row r="65" spans="1:6" ht="69.75" customHeight="1">
-      <c r="A65" s="239" t="s">
+      <c r="A65" s="222" t="s">
         <v>103</v>
       </c>
-      <c r="B65" s="239"/>
-      <c r="C65" s="239"/>
-      <c r="D65" s="239"/>
-      <c r="E65" s="239"/>
-      <c r="F65" s="239"/>
+      <c r="B65" s="222"/>
+      <c r="C65" s="222"/>
+      <c r="D65" s="222"/>
+      <c r="E65" s="222"/>
+      <c r="F65" s="222"/>
     </row>
     <row r="66" spans="1:6">
-      <c r="A66" s="239"/>
-      <c r="B66" s="239"/>
-      <c r="C66" s="239"/>
-      <c r="D66" s="239"/>
-      <c r="E66" s="239"/>
-      <c r="F66" s="239"/>
+      <c r="A66" s="222"/>
+      <c r="B66" s="222"/>
+      <c r="C66" s="222"/>
+      <c r="D66" s="222"/>
+      <c r="E66" s="222"/>
+      <c r="F66" s="222"/>
     </row>
     <row r="67" spans="1:6">
-      <c r="A67" s="239"/>
-      <c r="B67" s="239"/>
-      <c r="C67" s="239"/>
-      <c r="D67" s="239"/>
-      <c r="E67" s="239"/>
-      <c r="F67" s="239"/>
+      <c r="A67" s="222"/>
+      <c r="B67" s="222"/>
+      <c r="C67" s="222"/>
+      <c r="D67" s="222"/>
+      <c r="E67" s="222"/>
+      <c r="F67" s="222"/>
     </row>
     <row r="68" spans="1:6">
-      <c r="A68" s="239"/>
-      <c r="B68" s="239"/>
-      <c r="C68" s="239"/>
-      <c r="D68" s="239"/>
-      <c r="E68" s="239"/>
-      <c r="F68" s="239"/>
+      <c r="A68" s="222"/>
+      <c r="B68" s="222"/>
+      <c r="C68" s="222"/>
+      <c r="D68" s="222"/>
+      <c r="E68" s="222"/>
+      <c r="F68" s="222"/>
     </row>
     <row r="69" spans="1:6">
-      <c r="A69" s="242" t="s">
+      <c r="A69" s="224" t="s">
         <v>104</v>
       </c>
-      <c r="B69" s="242"/>
-      <c r="C69" s="242"/>
+      <c r="B69" s="224"/>
+      <c r="C69" s="224"/>
     </row>
     <row r="70" spans="1:6" ht="132" customHeight="1">
-      <c r="A70" s="239" t="s">
+      <c r="A70" s="222" t="s">
         <v>105</v>
       </c>
-      <c r="B70" s="239"/>
-      <c r="C70" s="239"/>
-      <c r="D70" s="239"/>
-      <c r="E70" s="239"/>
-      <c r="F70" s="239"/>
+      <c r="B70" s="222"/>
+      <c r="C70" s="222"/>
+      <c r="D70" s="222"/>
+      <c r="E70" s="222"/>
+      <c r="F70" s="222"/>
     </row>
     <row r="71" spans="1:6">
-      <c r="A71" s="242" t="s">
+      <c r="A71" s="224" t="s">
         <v>106</v>
       </c>
-      <c r="B71" s="242"/>
-      <c r="C71" s="242"/>
+      <c r="B71" s="224"/>
+      <c r="C71" s="224"/>
     </row>
     <row r="72" spans="1:6">
-      <c r="A72" s="238" t="s">
+      <c r="A72" s="223" t="s">
         <v>107</v>
       </c>
-      <c r="B72" s="239"/>
-      <c r="C72" s="239"/>
-      <c r="D72" s="239"/>
-      <c r="E72" s="239"/>
-      <c r="F72" s="239"/>
+      <c r="B72" s="222"/>
+      <c r="C72" s="222"/>
+      <c r="D72" s="222"/>
+      <c r="E72" s="222"/>
+      <c r="F72" s="222"/>
     </row>
     <row r="73" spans="1:6">
-      <c r="A73" s="239"/>
-      <c r="B73" s="239"/>
-      <c r="C73" s="239"/>
-      <c r="D73" s="239"/>
-      <c r="E73" s="239"/>
-      <c r="F73" s="239"/>
+      <c r="A73" s="222"/>
+      <c r="B73" s="222"/>
+      <c r="C73" s="222"/>
+      <c r="D73" s="222"/>
+      <c r="E73" s="222"/>
+      <c r="F73" s="222"/>
     </row>
     <row r="74" spans="1:6">
-      <c r="A74" s="239"/>
-      <c r="B74" s="239"/>
-      <c r="C74" s="239"/>
-      <c r="D74" s="239"/>
-      <c r="E74" s="239"/>
-      <c r="F74" s="239"/>
+      <c r="A74" s="222"/>
+      <c r="B74" s="222"/>
+      <c r="C74" s="222"/>
+      <c r="D74" s="222"/>
+      <c r="E74" s="222"/>
+      <c r="F74" s="222"/>
     </row>
     <row r="75" spans="1:6">
-      <c r="A75" s="243"/>
-      <c r="B75" s="243"/>
-      <c r="C75" s="243"/>
-      <c r="D75" s="243"/>
-      <c r="E75" s="243"/>
-      <c r="F75" s="243"/>
+      <c r="A75" s="221"/>
+      <c r="B75" s="221"/>
+      <c r="C75" s="221"/>
+      <c r="D75" s="221"/>
+      <c r="E75" s="221"/>
+      <c r="F75" s="221"/>
     </row>
     <row r="76" spans="1:6">
       <c r="A76"/>
@@ -11873,61 +11873,92 @@
       </c>
     </row>
     <row r="80" spans="1:6" ht="196.5" customHeight="1">
-      <c r="A80" s="221" t="s">
+      <c r="A80" s="236" t="s">
         <v>114</v>
       </c>
-      <c r="B80" s="221"/>
-      <c r="C80" s="221"/>
-      <c r="D80" s="221"/>
-      <c r="E80" s="221"/>
+      <c r="B80" s="236"/>
+      <c r="C80" s="236"/>
+      <c r="D80" s="236"/>
+      <c r="E80" s="236"/>
     </row>
     <row r="81" spans="1:5" ht="101.25" customHeight="1">
-      <c r="A81" s="221" t="s">
+      <c r="A81" s="236" t="s">
         <v>115</v>
       </c>
-      <c r="B81" s="221"/>
-      <c r="C81" s="221"/>
-      <c r="D81" s="221"/>
-      <c r="E81" s="221"/>
+      <c r="B81" s="236"/>
+      <c r="C81" s="236"/>
+      <c r="D81" s="236"/>
+      <c r="E81" s="236"/>
     </row>
     <row r="82" spans="1:5" ht="108" customHeight="1">
-      <c r="A82" s="221" t="s">
+      <c r="A82" s="236" t="s">
         <v>116</v>
       </c>
-      <c r="B82" s="221"/>
-      <c r="C82" s="221"/>
-      <c r="D82" s="221"/>
-      <c r="E82" s="221"/>
+      <c r="B82" s="236"/>
+      <c r="C82" s="236"/>
+      <c r="D82" s="236"/>
+      <c r="E82" s="236"/>
     </row>
     <row r="83" spans="1:5" ht="66" customHeight="1">
-      <c r="A83" s="221" t="s">
+      <c r="A83" s="236" t="s">
         <v>117</v>
       </c>
-      <c r="B83" s="221"/>
-      <c r="C83" s="221"/>
-      <c r="D83" s="221"/>
-      <c r="E83" s="221"/>
+      <c r="B83" s="236"/>
+      <c r="C83" s="236"/>
+      <c r="D83" s="236"/>
+      <c r="E83" s="236"/>
     </row>
     <row r="84" spans="1:5" ht="66" customHeight="1">
-      <c r="A84" s="221" t="s">
+      <c r="A84" s="236" t="s">
         <v>118</v>
       </c>
-      <c r="B84" s="221"/>
-      <c r="C84" s="221"/>
-      <c r="D84" s="221"/>
-      <c r="E84" s="221"/>
+      <c r="B84" s="236"/>
+      <c r="C84" s="236"/>
+      <c r="D84" s="236"/>
+      <c r="E84" s="236"/>
     </row>
     <row r="85" spans="1:5" ht="66.75" customHeight="1">
-      <c r="A85" s="221" t="s">
+      <c r="A85" s="236" t="s">
         <v>119</v>
       </c>
-      <c r="B85" s="221"/>
-      <c r="C85" s="221"/>
-      <c r="D85" s="221"/>
-      <c r="E85" s="221"/>
+      <c r="B85" s="236"/>
+      <c r="C85" s="236"/>
+      <c r="D85" s="236"/>
+      <c r="E85" s="236"/>
     </row>
   </sheetData>
   <mergeCells count="47">
+    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="A29:F29"/>
+    <mergeCell ref="A30:F30"/>
+    <mergeCell ref="A28:F28"/>
+    <mergeCell ref="A85:E85"/>
+    <mergeCell ref="A80:E80"/>
+    <mergeCell ref="A81:E81"/>
+    <mergeCell ref="A82:E82"/>
+    <mergeCell ref="A83:E83"/>
+    <mergeCell ref="A84:E84"/>
+    <mergeCell ref="A34:F34"/>
+    <mergeCell ref="A44:F44"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A37:E37"/>
+    <mergeCell ref="A31:E31"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="A35:F35"/>
+    <mergeCell ref="A32:F32"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A72:F72"/>
+    <mergeCell ref="A45:F45"/>
+    <mergeCell ref="A46:F46"/>
+    <mergeCell ref="A47:F47"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="A58:G58"/>
+    <mergeCell ref="A57:C57"/>
+    <mergeCell ref="A40:F40"/>
+    <mergeCell ref="A41:F41"/>
+    <mergeCell ref="A42:F42"/>
+    <mergeCell ref="A43:F43"/>
+    <mergeCell ref="A38:D38"/>
     <mergeCell ref="A75:F75"/>
     <mergeCell ref="A59:F59"/>
     <mergeCell ref="A60:F60"/>
@@ -11944,48 +11975,17 @@
     <mergeCell ref="A70:F70"/>
     <mergeCell ref="A71:C71"/>
     <mergeCell ref="A73:F73"/>
-    <mergeCell ref="A35:F35"/>
-    <mergeCell ref="A32:F32"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A72:F72"/>
-    <mergeCell ref="A45:F45"/>
-    <mergeCell ref="A46:F46"/>
-    <mergeCell ref="A47:F47"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="A58:G58"/>
-    <mergeCell ref="A57:C57"/>
-    <mergeCell ref="A40:F40"/>
-    <mergeCell ref="A41:F41"/>
-    <mergeCell ref="A42:F42"/>
-    <mergeCell ref="A43:F43"/>
-    <mergeCell ref="A38:D38"/>
-    <mergeCell ref="A26:E26"/>
-    <mergeCell ref="A29:F29"/>
-    <mergeCell ref="A30:F30"/>
-    <mergeCell ref="A28:F28"/>
-    <mergeCell ref="A85:E85"/>
-    <mergeCell ref="A80:E80"/>
-    <mergeCell ref="A81:E81"/>
-    <mergeCell ref="A82:E82"/>
-    <mergeCell ref="A83:E83"/>
-    <mergeCell ref="A84:E84"/>
-    <mergeCell ref="A34:F34"/>
-    <mergeCell ref="A44:F44"/>
-    <mergeCell ref="A36:D36"/>
-    <mergeCell ref="A37:E37"/>
-    <mergeCell ref="A31:E31"/>
-    <mergeCell ref="A39:C39"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E39" r:id="rId1"/>
-    <hyperlink ref="A72" r:id="rId2"/>
-    <hyperlink ref="A60" r:id="rId3"/>
-    <hyperlink ref="F20" r:id="rId4" location="Shortcut_rule"/>
-    <hyperlink ref="A61" r:id="rId5"/>
-    <hyperlink ref="A62" r:id="rId6"/>
-    <hyperlink ref="A63" r:id="rId7"/>
-    <hyperlink ref="A28" r:id="rId8"/>
-    <hyperlink ref="A29" r:id="rId9"/>
+    <hyperlink ref="E39" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A72" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A60" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="F20" r:id="rId4" location="Shortcut_rule" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="A61" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="A62" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="A63" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="A28" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="A29" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId10"/>
@@ -11993,7 +11993,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:W85"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
@@ -13035,8 +13035,8 @@
     <mergeCell ref="A53:E53"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B54" r:id="rId1"/>
-    <hyperlink ref="A35" r:id="rId2"/>
+    <hyperlink ref="B54" r:id="rId1" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
+    <hyperlink ref="A35" r:id="rId2" xr:uid="{00000000-0004-0000-0900-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -13045,11 +13045,11 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:T39"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
@@ -13062,22 +13062,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
-      <c r="A1" s="278" t="s">
+      <c r="A1" s="279" t="s">
         <v>1072</v>
       </c>
-      <c r="B1" s="221"/>
-      <c r="C1" s="221"/>
-      <c r="D1" s="221"/>
-      <c r="E1" s="221"/>
-      <c r="F1" s="221"/>
-      <c r="G1" s="221"/>
-      <c r="H1" s="221"/>
-      <c r="I1" s="221"/>
-      <c r="J1" s="221"/>
-      <c r="K1" s="221"/>
-      <c r="L1" s="221"/>
-      <c r="M1" s="221"/>
-      <c r="N1" s="221"/>
+      <c r="B1" s="236"/>
+      <c r="C1" s="236"/>
+      <c r="D1" s="236"/>
+      <c r="E1" s="236"/>
+      <c r="F1" s="236"/>
+      <c r="G1" s="236"/>
+      <c r="H1" s="236"/>
+      <c r="I1" s="236"/>
+      <c r="J1" s="236"/>
+      <c r="K1" s="236"/>
+      <c r="L1" s="236"/>
+      <c r="M1" s="236"/>
+      <c r="N1" s="236"/>
       <c r="O1" s="186"/>
       <c r="P1" s="186"/>
       <c r="Q1" s="186"/>
@@ -13086,22 +13086,22 @@
       <c r="T1" s="186"/>
     </row>
     <row r="2" spans="1:20">
-      <c r="A2" s="221" t="s">
+      <c r="A2" s="236" t="s">
         <v>1073</v>
       </c>
-      <c r="B2" s="221"/>
-      <c r="C2" s="221"/>
-      <c r="D2" s="221"/>
-      <c r="E2" s="221"/>
-      <c r="F2" s="221"/>
-      <c r="G2" s="221"/>
-      <c r="H2" s="221"/>
-      <c r="I2" s="221"/>
-      <c r="J2" s="221"/>
-      <c r="K2" s="221"/>
-      <c r="L2" s="221"/>
-      <c r="M2" s="221"/>
-      <c r="N2" s="221"/>
+      <c r="B2" s="236"/>
+      <c r="C2" s="236"/>
+      <c r="D2" s="236"/>
+      <c r="E2" s="236"/>
+      <c r="F2" s="236"/>
+      <c r="G2" s="236"/>
+      <c r="H2" s="236"/>
+      <c r="I2" s="236"/>
+      <c r="J2" s="236"/>
+      <c r="K2" s="236"/>
+      <c r="L2" s="236"/>
+      <c r="M2" s="236"/>
+      <c r="N2" s="236"/>
       <c r="O2" s="186"/>
       <c r="P2" s="186"/>
       <c r="Q2" s="186"/>
@@ -13110,22 +13110,22 @@
       <c r="T2" s="186"/>
     </row>
     <row r="3" spans="1:20">
-      <c r="A3" s="221" t="s">
+      <c r="A3" s="236" t="s">
         <v>1074</v>
       </c>
-      <c r="B3" s="221"/>
-      <c r="C3" s="221"/>
-      <c r="D3" s="221"/>
-      <c r="E3" s="221"/>
-      <c r="F3" s="221"/>
-      <c r="G3" s="221"/>
-      <c r="H3" s="221"/>
-      <c r="I3" s="221"/>
-      <c r="J3" s="221"/>
-      <c r="K3" s="221"/>
-      <c r="L3" s="221"/>
-      <c r="M3" s="221"/>
-      <c r="N3" s="221"/>
+      <c r="B3" s="236"/>
+      <c r="C3" s="236"/>
+      <c r="D3" s="236"/>
+      <c r="E3" s="236"/>
+      <c r="F3" s="236"/>
+      <c r="G3" s="236"/>
+      <c r="H3" s="236"/>
+      <c r="I3" s="236"/>
+      <c r="J3" s="236"/>
+      <c r="K3" s="236"/>
+      <c r="L3" s="236"/>
+      <c r="M3" s="236"/>
+      <c r="N3" s="236"/>
       <c r="O3" s="186"/>
       <c r="P3" s="186"/>
       <c r="Q3" s="186"/>
@@ -13148,14 +13148,14 @@
       <c r="L4" s="186"/>
       <c r="M4" s="186"/>
       <c r="N4" s="186"/>
-      <c r="O4" s="221" t="s">
+      <c r="O4" s="236" t="s">
         <v>1075</v>
       </c>
-      <c r="P4" s="221"/>
-      <c r="Q4" s="221"/>
-      <c r="R4" s="221"/>
-      <c r="S4" s="221"/>
-      <c r="T4" s="221"/>
+      <c r="P4" s="236"/>
+      <c r="Q4" s="236"/>
+      <c r="R4" s="236"/>
+      <c r="S4" s="236"/>
+      <c r="T4" s="236"/>
     </row>
     <row r="5" spans="1:20">
       <c r="A5" s="186"/>
@@ -13172,32 +13172,32 @@
       <c r="L5" s="186"/>
       <c r="M5" s="186"/>
       <c r="N5" s="186"/>
-      <c r="O5" s="221" t="s">
+      <c r="O5" s="236" t="s">
         <v>1076</v>
       </c>
-      <c r="P5" s="221"/>
-      <c r="Q5" s="221"/>
-      <c r="R5" s="221"/>
-      <c r="S5" s="221"/>
-      <c r="T5" s="221"/>
+      <c r="P5" s="236"/>
+      <c r="Q5" s="236"/>
+      <c r="R5" s="236"/>
+      <c r="S5" s="236"/>
+      <c r="T5" s="236"/>
     </row>
     <row r="6" spans="1:20">
-      <c r="A6" s="239" t="s">
+      <c r="A6" s="222" t="s">
         <v>1077</v>
       </c>
-      <c r="B6" s="239"/>
-      <c r="C6" s="239"/>
-      <c r="D6" s="239"/>
-      <c r="E6" s="239"/>
-      <c r="F6" s="239"/>
-      <c r="G6" s="239"/>
-      <c r="H6" s="239"/>
-      <c r="I6" s="239"/>
-      <c r="J6" s="239"/>
-      <c r="K6" s="239"/>
-      <c r="L6" s="239"/>
-      <c r="M6" s="239"/>
-      <c r="N6" s="239"/>
+      <c r="B6" s="222"/>
+      <c r="C6" s="222"/>
+      <c r="D6" s="222"/>
+      <c r="E6" s="222"/>
+      <c r="F6" s="222"/>
+      <c r="G6" s="222"/>
+      <c r="H6" s="222"/>
+      <c r="I6" s="222"/>
+      <c r="J6" s="222"/>
+      <c r="K6" s="222"/>
+      <c r="L6" s="222"/>
+      <c r="M6" s="222"/>
+      <c r="N6" s="222"/>
       <c r="O6" s="186"/>
       <c r="P6" s="186"/>
       <c r="Q6" s="186"/>
@@ -13206,22 +13206,22 @@
       <c r="T6" s="186"/>
     </row>
     <row r="11" spans="1:20">
-      <c r="A11" s="221" t="s">
+      <c r="A11" s="236" t="s">
         <v>1078</v>
       </c>
-      <c r="B11" s="221"/>
-      <c r="C11" s="221"/>
-      <c r="D11" s="221"/>
-      <c r="E11" s="221"/>
-      <c r="F11" s="221"/>
-      <c r="G11" s="221"/>
-      <c r="H11" s="221"/>
-      <c r="I11" s="221"/>
-      <c r="J11" s="221"/>
-      <c r="K11" s="221"/>
-      <c r="L11" s="221"/>
-      <c r="M11" s="221"/>
-      <c r="N11" s="221"/>
+      <c r="B11" s="236"/>
+      <c r="C11" s="236"/>
+      <c r="D11" s="236"/>
+      <c r="E11" s="236"/>
+      <c r="F11" s="236"/>
+      <c r="G11" s="236"/>
+      <c r="H11" s="236"/>
+      <c r="I11" s="236"/>
+      <c r="J11" s="236"/>
+      <c r="K11" s="236"/>
+      <c r="L11" s="236"/>
+      <c r="M11" s="236"/>
+      <c r="N11" s="236"/>
       <c r="O11" s="186"/>
       <c r="P11" s="186"/>
       <c r="Q11" s="186"/>
@@ -13230,22 +13230,22 @@
       <c r="T11" s="186"/>
     </row>
     <row r="12" spans="1:20">
-      <c r="A12" s="221" t="s">
+      <c r="A12" s="236" t="s">
         <v>1079</v>
       </c>
-      <c r="B12" s="221"/>
-      <c r="C12" s="221"/>
-      <c r="D12" s="221"/>
-      <c r="E12" s="221"/>
-      <c r="F12" s="221"/>
-      <c r="G12" s="221"/>
-      <c r="H12" s="221"/>
-      <c r="I12" s="221"/>
-      <c r="J12" s="221"/>
-      <c r="K12" s="221"/>
-      <c r="L12" s="221"/>
-      <c r="M12" s="221"/>
-      <c r="N12" s="221"/>
+      <c r="B12" s="236"/>
+      <c r="C12" s="236"/>
+      <c r="D12" s="236"/>
+      <c r="E12" s="236"/>
+      <c r="F12" s="236"/>
+      <c r="G12" s="236"/>
+      <c r="H12" s="236"/>
+      <c r="I12" s="236"/>
+      <c r="J12" s="236"/>
+      <c r="K12" s="236"/>
+      <c r="L12" s="236"/>
+      <c r="M12" s="236"/>
+      <c r="N12" s="236"/>
       <c r="O12" s="186"/>
       <c r="P12" s="186"/>
       <c r="Q12" s="186"/>
@@ -13254,22 +13254,22 @@
       <c r="T12" s="186"/>
     </row>
     <row r="13" spans="1:20">
-      <c r="A13" s="221" t="s">
+      <c r="A13" s="236" t="s">
         <v>1080</v>
       </c>
-      <c r="B13" s="221"/>
-      <c r="C13" s="221"/>
-      <c r="D13" s="221"/>
-      <c r="E13" s="221"/>
-      <c r="F13" s="221"/>
-      <c r="G13" s="221"/>
-      <c r="H13" s="221"/>
-      <c r="I13" s="221"/>
-      <c r="J13" s="221"/>
-      <c r="K13" s="221"/>
-      <c r="L13" s="221"/>
-      <c r="M13" s="221"/>
-      <c r="N13" s="221"/>
+      <c r="B13" s="236"/>
+      <c r="C13" s="236"/>
+      <c r="D13" s="236"/>
+      <c r="E13" s="236"/>
+      <c r="F13" s="236"/>
+      <c r="G13" s="236"/>
+      <c r="H13" s="236"/>
+      <c r="I13" s="236"/>
+      <c r="J13" s="236"/>
+      <c r="K13" s="236"/>
+      <c r="L13" s="236"/>
+      <c r="M13" s="236"/>
+      <c r="N13" s="236"/>
       <c r="O13"/>
       <c r="P13" s="186"/>
       <c r="Q13" s="186"/>
@@ -13302,22 +13302,22 @@
       <c r="T14" s="186"/>
     </row>
     <row r="15" spans="1:20">
-      <c r="A15" s="221" t="s">
+      <c r="A15" s="236" t="s">
         <v>1082</v>
       </c>
-      <c r="B15" s="221"/>
-      <c r="C15" s="221"/>
-      <c r="D15" s="221"/>
-      <c r="E15" s="221"/>
-      <c r="F15" s="221"/>
-      <c r="G15" s="221"/>
-      <c r="H15" s="221"/>
-      <c r="I15" s="221"/>
-      <c r="J15" s="221"/>
-      <c r="K15" s="221"/>
-      <c r="L15" s="221"/>
-      <c r="M15" s="221"/>
-      <c r="N15" s="221"/>
+      <c r="B15" s="236"/>
+      <c r="C15" s="236"/>
+      <c r="D15" s="236"/>
+      <c r="E15" s="236"/>
+      <c r="F15" s="236"/>
+      <c r="G15" s="236"/>
+      <c r="H15" s="236"/>
+      <c r="I15" s="236"/>
+      <c r="J15" s="236"/>
+      <c r="K15" s="236"/>
+      <c r="L15" s="236"/>
+      <c r="M15" s="236"/>
+      <c r="N15" s="236"/>
       <c r="O15"/>
       <c r="P15" s="186"/>
       <c r="Q15" s="186"/>
@@ -13326,20 +13326,20 @@
       <c r="T15" s="186"/>
     </row>
     <row r="16" spans="1:20">
-      <c r="A16" s="221"/>
-      <c r="B16" s="221"/>
-      <c r="C16" s="221"/>
-      <c r="D16" s="221"/>
-      <c r="E16" s="221"/>
-      <c r="F16" s="221"/>
-      <c r="G16" s="221"/>
-      <c r="H16" s="221"/>
-      <c r="I16" s="221"/>
-      <c r="J16" s="221"/>
-      <c r="K16" s="221"/>
-      <c r="L16" s="221"/>
-      <c r="M16" s="221"/>
-      <c r="N16" s="221"/>
+      <c r="A16" s="236"/>
+      <c r="B16" s="236"/>
+      <c r="C16" s="236"/>
+      <c r="D16" s="236"/>
+      <c r="E16" s="236"/>
+      <c r="F16" s="236"/>
+      <c r="G16" s="236"/>
+      <c r="H16" s="236"/>
+      <c r="I16" s="236"/>
+      <c r="J16" s="236"/>
+      <c r="K16" s="236"/>
+      <c r="L16" s="236"/>
+      <c r="M16" s="236"/>
+      <c r="N16" s="236"/>
       <c r="O16"/>
       <c r="P16" s="186"/>
       <c r="Q16" s="186"/>
@@ -13348,40 +13348,40 @@
       <c r="T16" s="186"/>
     </row>
     <row r="17" spans="1:14">
-      <c r="A17" s="221" t="s">
+      <c r="A17" s="236" t="s">
         <v>1083</v>
       </c>
-      <c r="B17" s="221"/>
-      <c r="C17" s="221"/>
-      <c r="D17" s="221"/>
-      <c r="E17" s="221"/>
-      <c r="F17" s="221"/>
-      <c r="G17" s="221"/>
-      <c r="H17" s="221"/>
-      <c r="I17" s="221"/>
-      <c r="J17" s="221"/>
-      <c r="K17" s="221"/>
-      <c r="L17" s="221"/>
-      <c r="M17" s="221"/>
-      <c r="N17" s="221"/>
+      <c r="B17" s="236"/>
+      <c r="C17" s="236"/>
+      <c r="D17" s="236"/>
+      <c r="E17" s="236"/>
+      <c r="F17" s="236"/>
+      <c r="G17" s="236"/>
+      <c r="H17" s="236"/>
+      <c r="I17" s="236"/>
+      <c r="J17" s="236"/>
+      <c r="K17" s="236"/>
+      <c r="L17" s="236"/>
+      <c r="M17" s="236"/>
+      <c r="N17" s="236"/>
     </row>
     <row r="18" spans="1:14">
-      <c r="A18" s="221" t="s">
+      <c r="A18" s="236" t="s">
         <v>1084</v>
       </c>
-      <c r="B18" s="221"/>
-      <c r="C18" s="221"/>
-      <c r="D18" s="221"/>
-      <c r="E18" s="221"/>
-      <c r="F18" s="221"/>
-      <c r="G18" s="221"/>
-      <c r="H18" s="221"/>
-      <c r="I18" s="221"/>
-      <c r="J18" s="221"/>
-      <c r="K18" s="221"/>
-      <c r="L18" s="221"/>
-      <c r="M18" s="221"/>
-      <c r="N18" s="221"/>
+      <c r="B18" s="236"/>
+      <c r="C18" s="236"/>
+      <c r="D18" s="236"/>
+      <c r="E18" s="236"/>
+      <c r="F18" s="236"/>
+      <c r="G18" s="236"/>
+      <c r="H18" s="236"/>
+      <c r="I18" s="236"/>
+      <c r="J18" s="236"/>
+      <c r="K18" s="236"/>
+      <c r="L18" s="236"/>
+      <c r="M18" s="236"/>
+      <c r="N18" s="236"/>
     </row>
     <row r="19" spans="1:14">
       <c r="A19"/>
@@ -13483,29 +13483,29 @@
       <c r="A27" s="186" t="s">
         <v>1085</v>
       </c>
-      <c r="B27" s="221" t="s">
+      <c r="B27" s="236" t="s">
         <v>1086</v>
       </c>
-      <c r="C27" s="221"/>
-      <c r="D27" s="221"/>
-      <c r="E27" s="221"/>
-      <c r="F27" s="221"/>
-      <c r="G27" s="221"/>
-      <c r="H27" s="221"/>
-      <c r="I27" s="221"/>
-      <c r="J27" s="221"/>
-      <c r="K27" s="221"/>
-      <c r="L27" s="221"/>
-      <c r="M27" s="221"/>
-      <c r="N27" s="221"/>
+      <c r="C27" s="236"/>
+      <c r="D27" s="236"/>
+      <c r="E27" s="236"/>
+      <c r="F27" s="236"/>
+      <c r="G27" s="236"/>
+      <c r="H27" s="236"/>
+      <c r="I27" s="236"/>
+      <c r="J27" s="236"/>
+      <c r="K27" s="236"/>
+      <c r="L27" s="236"/>
+      <c r="M27" s="236"/>
+      <c r="N27" s="236"/>
     </row>
     <row r="29" spans="1:14">
-      <c r="A29" s="279" t="s">
+      <c r="A29" s="278" t="s">
         <v>59</v>
       </c>
-      <c r="B29" s="279"/>
-      <c r="C29" s="279"/>
-      <c r="D29" s="279"/>
+      <c r="B29" s="278"/>
+      <c r="C29" s="278"/>
+      <c r="D29" s="278"/>
       <c r="E29" s="186"/>
       <c r="F29" s="186"/>
       <c r="G29" s="186"/>
@@ -13627,16 +13627,26 @@
       <c r="E37" s="186"/>
     </row>
     <row r="39" spans="1:5" ht="51.75" customHeight="1">
-      <c r="A39" s="221" t="s">
+      <c r="A39" s="236" t="s">
         <v>1099</v>
       </c>
-      <c r="B39" s="221"/>
-      <c r="C39" s="221"/>
-      <c r="D39" s="221"/>
+      <c r="B39" s="236"/>
+      <c r="C39" s="236"/>
+      <c r="D39" s="236"/>
       <c r="E39" s="186"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="O4:T4"/>
+    <mergeCell ref="O5:T5"/>
+    <mergeCell ref="A2:N2"/>
+    <mergeCell ref="A3:N3"/>
+    <mergeCell ref="A6:N6"/>
+    <mergeCell ref="A11:N11"/>
+    <mergeCell ref="A12:N12"/>
+    <mergeCell ref="A13:N13"/>
+    <mergeCell ref="A14:N14"/>
+    <mergeCell ref="A1:N1"/>
     <mergeCell ref="A29:D29"/>
     <mergeCell ref="A39:D39"/>
     <mergeCell ref="B27:N27"/>
@@ -13644,19 +13654,9 @@
     <mergeCell ref="A16:N16"/>
     <mergeCell ref="A17:N17"/>
     <mergeCell ref="A18:N18"/>
-    <mergeCell ref="A11:N11"/>
-    <mergeCell ref="A12:N12"/>
-    <mergeCell ref="A13:N13"/>
-    <mergeCell ref="A14:N14"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="O4:T4"/>
-    <mergeCell ref="O5:T5"/>
-    <mergeCell ref="A2:N2"/>
-    <mergeCell ref="A3:N3"/>
-    <mergeCell ref="A6:N6"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1"/>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -13665,14 +13665,14 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:K57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="8" ySplit="1" topLeftCell="I26" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="8" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B55" sqref="B55"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -14734,23 +14734,23 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B17" r:id="rId1"/>
-    <hyperlink ref="E17" r:id="rId2"/>
-    <hyperlink ref="B18" r:id="rId3"/>
-    <hyperlink ref="B19" r:id="rId4"/>
-    <hyperlink ref="B48" r:id="rId5"/>
-    <hyperlink ref="B5" r:id="rId6"/>
-    <hyperlink ref="B6" r:id="rId7"/>
-    <hyperlink ref="B12" r:id="rId8"/>
-    <hyperlink ref="C12" r:id="rId9" tooltip="Heuristic (computer science)" display="https://en.wikipedia.org/wiki/Heuristic_(computer_science)"/>
-    <hyperlink ref="B7" r:id="rId10"/>
-    <hyperlink ref="B23" r:id="rId11"/>
-    <hyperlink ref="B14" r:id="rId12"/>
-    <hyperlink ref="B8" r:id="rId13" tooltip="Viterbi algorithm" display="https://en.wikipedia.org/wiki/Viterbi_algorithm"/>
-    <hyperlink ref="B9" r:id="rId14"/>
-    <hyperlink ref="B10" r:id="rId15" location="CITEREFThorup2004"/>
-    <hyperlink ref="B15" r:id="rId16"/>
-    <hyperlink ref="B55" r:id="rId17"/>
+    <hyperlink ref="B17" r:id="rId1" xr:uid="{00000000-0004-0000-0B00-000000000000}"/>
+    <hyperlink ref="E17" r:id="rId2" xr:uid="{00000000-0004-0000-0B00-000001000000}"/>
+    <hyperlink ref="B18" r:id="rId3" xr:uid="{00000000-0004-0000-0B00-000002000000}"/>
+    <hyperlink ref="B19" r:id="rId4" xr:uid="{00000000-0004-0000-0B00-000003000000}"/>
+    <hyperlink ref="B48" r:id="rId5" xr:uid="{00000000-0004-0000-0B00-000004000000}"/>
+    <hyperlink ref="B5" r:id="rId6" xr:uid="{00000000-0004-0000-0B00-000005000000}"/>
+    <hyperlink ref="B6" r:id="rId7" xr:uid="{00000000-0004-0000-0B00-000006000000}"/>
+    <hyperlink ref="B12" r:id="rId8" xr:uid="{00000000-0004-0000-0B00-000007000000}"/>
+    <hyperlink ref="C12" r:id="rId9" tooltip="Heuristic (computer science)" display="https://en.wikipedia.org/wiki/Heuristic_(computer_science)" xr:uid="{00000000-0004-0000-0B00-000008000000}"/>
+    <hyperlink ref="B7" r:id="rId10" xr:uid="{00000000-0004-0000-0B00-000009000000}"/>
+    <hyperlink ref="B23" r:id="rId11" xr:uid="{00000000-0004-0000-0B00-00000A000000}"/>
+    <hyperlink ref="B14" r:id="rId12" xr:uid="{00000000-0004-0000-0B00-00000B000000}"/>
+    <hyperlink ref="B8" r:id="rId13" tooltip="Viterbi algorithm" display="https://en.wikipedia.org/wiki/Viterbi_algorithm" xr:uid="{00000000-0004-0000-0B00-00000C000000}"/>
+    <hyperlink ref="B9" r:id="rId14" xr:uid="{00000000-0004-0000-0B00-00000D000000}"/>
+    <hyperlink ref="B10" r:id="rId15" location="CITEREFThorup2004" xr:uid="{00000000-0004-0000-0B00-00000E000000}"/>
+    <hyperlink ref="B15" r:id="rId16" xr:uid="{00000000-0004-0000-0B00-00000F000000}"/>
+    <hyperlink ref="B55" r:id="rId17" xr:uid="{00000000-0004-0000-0B00-000010000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId18"/>
@@ -14758,10 +14758,10 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -14813,7 +14813,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:A79"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -14916,7 +14916,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A9" r:id="rId1"/>
+    <hyperlink ref="A9" r:id="rId1" xr:uid="{00000000-0004-0000-0D00-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -14924,7 +14924,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R86"/>
   <sheetViews>
     <sheetView topLeftCell="A55" workbookViewId="0">
@@ -14967,15 +14967,15 @@
       <c r="H1" s="164"/>
       <c r="I1" s="164"/>
       <c r="J1" s="164"/>
-      <c r="L1" s="249" t="s">
+      <c r="L1" s="244" t="s">
         <v>126</v>
       </c>
-      <c r="M1" s="244"/>
-      <c r="N1" s="244"/>
-      <c r="O1" s="244"/>
-      <c r="P1" s="244"/>
-      <c r="Q1" s="244"/>
-      <c r="R1" s="244"/>
+      <c r="M1" s="245"/>
+      <c r="N1" s="245"/>
+      <c r="O1" s="245"/>
+      <c r="P1" s="245"/>
+      <c r="Q1" s="245"/>
+      <c r="R1" s="245"/>
     </row>
     <row r="2" spans="1:18" s="4" customFormat="1" ht="15.75">
       <c r="A2" s="165" t="s">
@@ -15533,15 +15533,15 @@
       <c r="J21" s="142"/>
     </row>
     <row r="22" spans="1:12" ht="45" customHeight="1">
-      <c r="A22" s="247" t="s">
+      <c r="A22" s="246" t="s">
         <v>149</v>
       </c>
-      <c r="B22" s="247"/>
-      <c r="C22" s="247"/>
-      <c r="D22" s="247"/>
-      <c r="E22" s="247"/>
-      <c r="F22" s="247"/>
-      <c r="G22" s="247"/>
+      <c r="B22" s="246"/>
+      <c r="C22" s="246"/>
+      <c r="D22" s="246"/>
+      <c r="E22" s="246"/>
+      <c r="F22" s="246"/>
+      <c r="G22" s="246"/>
       <c r="H22" s="166"/>
       <c r="I22" s="166"/>
       <c r="J22" s="166"/>
@@ -15552,15 +15552,15 @@
       <c r="A23" s="39"/>
     </row>
     <row r="24" spans="1:12">
-      <c r="A24" s="244" t="s">
+      <c r="A24" s="245" t="s">
         <v>150</v>
       </c>
-      <c r="B24" s="244"/>
-      <c r="C24" s="244"/>
-      <c r="D24" s="244"/>
-      <c r="E24" s="244"/>
-      <c r="F24" s="244"/>
-      <c r="G24" s="244"/>
+      <c r="B24" s="245"/>
+      <c r="C24" s="245"/>
+      <c r="D24" s="245"/>
+      <c r="E24" s="245"/>
+      <c r="F24" s="245"/>
+      <c r="G24" s="245"/>
       <c r="H24" s="191"/>
       <c r="I24" s="191"/>
       <c r="J24" s="191"/>
@@ -15599,127 +15599,127 @@
       <c r="J28" s="6"/>
     </row>
     <row r="29" spans="1:12">
-      <c r="A29" s="221" t="s">
+      <c r="A29" s="236" t="s">
         <v>153</v>
       </c>
-      <c r="B29" s="221"/>
-      <c r="C29" s="221"/>
-      <c r="D29" s="221"/>
-      <c r="E29" s="221"/>
-      <c r="F29" s="221"/>
-      <c r="G29" s="221"/>
+      <c r="B29" s="236"/>
+      <c r="C29" s="236"/>
+      <c r="D29" s="236"/>
+      <c r="E29" s="236"/>
+      <c r="F29" s="236"/>
+      <c r="G29" s="236"/>
       <c r="H29" s="186"/>
       <c r="I29" s="186"/>
       <c r="J29" s="186"/>
     </row>
     <row r="30" spans="1:12">
-      <c r="A30" s="221" t="s">
+      <c r="A30" s="236" t="s">
         <v>154</v>
       </c>
-      <c r="B30" s="221"/>
-      <c r="C30" s="221"/>
-      <c r="D30" s="221"/>
-      <c r="E30" s="221"/>
-      <c r="F30" s="221"/>
-      <c r="G30" s="221"/>
+      <c r="B30" s="236"/>
+      <c r="C30" s="236"/>
+      <c r="D30" s="236"/>
+      <c r="E30" s="236"/>
+      <c r="F30" s="236"/>
+      <c r="G30" s="236"/>
       <c r="H30" s="186"/>
       <c r="I30" s="186"/>
       <c r="J30" s="186"/>
     </row>
     <row r="31" spans="1:12">
-      <c r="A31" s="248" t="s">
+      <c r="A31" s="250" t="s">
         <v>155</v>
       </c>
-      <c r="B31" s="248"/>
-      <c r="C31" s="248"/>
-      <c r="D31" s="248"/>
-      <c r="E31" s="248"/>
-      <c r="F31" s="248"/>
-      <c r="G31" s="248"/>
+      <c r="B31" s="250"/>
+      <c r="C31" s="250"/>
+      <c r="D31" s="250"/>
+      <c r="E31" s="250"/>
+      <c r="F31" s="250"/>
+      <c r="G31" s="250"/>
       <c r="H31" s="189"/>
       <c r="I31" s="189"/>
       <c r="J31" s="189"/>
     </row>
     <row r="32" spans="1:12">
-      <c r="A32" s="248" t="s">
+      <c r="A32" s="250" t="s">
         <v>156</v>
       </c>
-      <c r="B32" s="248"/>
-      <c r="C32" s="248"/>
-      <c r="D32" s="248"/>
-      <c r="E32" s="248"/>
-      <c r="F32" s="248"/>
-      <c r="G32" s="248"/>
+      <c r="B32" s="250"/>
+      <c r="C32" s="250"/>
+      <c r="D32" s="250"/>
+      <c r="E32" s="250"/>
+      <c r="F32" s="250"/>
+      <c r="G32" s="250"/>
       <c r="H32" s="189"/>
       <c r="I32" s="189"/>
       <c r="J32" s="189"/>
     </row>
     <row r="33" spans="1:10">
-      <c r="A33" s="248" t="s">
+      <c r="A33" s="250" t="s">
         <v>157</v>
       </c>
-      <c r="B33" s="248"/>
-      <c r="C33" s="248"/>
-      <c r="D33" s="248"/>
-      <c r="E33" s="248"/>
-      <c r="F33" s="248"/>
-      <c r="G33" s="248"/>
+      <c r="B33" s="250"/>
+      <c r="C33" s="250"/>
+      <c r="D33" s="250"/>
+      <c r="E33" s="250"/>
+      <c r="F33" s="250"/>
+      <c r="G33" s="250"/>
       <c r="H33" s="189"/>
       <c r="I33" s="189"/>
       <c r="J33" s="189"/>
     </row>
     <row r="34" spans="1:10">
-      <c r="A34" s="248" t="s">
+      <c r="A34" s="250" t="s">
         <v>158</v>
       </c>
-      <c r="B34" s="248"/>
-      <c r="C34" s="248"/>
-      <c r="D34" s="248"/>
-      <c r="E34" s="248"/>
-      <c r="F34" s="248"/>
-      <c r="G34" s="248"/>
+      <c r="B34" s="250"/>
+      <c r="C34" s="250"/>
+      <c r="D34" s="250"/>
+      <c r="E34" s="250"/>
+      <c r="F34" s="250"/>
+      <c r="G34" s="250"/>
       <c r="H34" s="189"/>
       <c r="I34" s="189"/>
       <c r="J34" s="189"/>
     </row>
     <row r="36" spans="1:10">
-      <c r="A36" s="248" t="s">
+      <c r="A36" s="250" t="s">
         <v>159</v>
       </c>
-      <c r="B36" s="248"/>
-      <c r="C36" s="248"/>
-      <c r="D36" s="248"/>
-      <c r="E36" s="248"/>
-      <c r="F36" s="248"/>
-      <c r="G36" s="248"/>
+      <c r="B36" s="250"/>
+      <c r="C36" s="250"/>
+      <c r="D36" s="250"/>
+      <c r="E36" s="250"/>
+      <c r="F36" s="250"/>
+      <c r="G36" s="250"/>
       <c r="H36" s="189"/>
       <c r="I36" s="189"/>
       <c r="J36" s="189"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="248" t="s">
+      <c r="A37" s="250" t="s">
         <v>160</v>
       </c>
-      <c r="B37" s="248"/>
-      <c r="C37" s="248"/>
-      <c r="D37" s="248"/>
-      <c r="E37" s="248"/>
-      <c r="F37" s="248"/>
-      <c r="G37" s="248"/>
+      <c r="B37" s="250"/>
+      <c r="C37" s="250"/>
+      <c r="D37" s="250"/>
+      <c r="E37" s="250"/>
+      <c r="F37" s="250"/>
+      <c r="G37" s="250"/>
       <c r="H37" s="189"/>
       <c r="I37" s="189"/>
       <c r="J37" s="189"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="248" t="s">
+      <c r="A38" s="250" t="s">
         <v>161</v>
       </c>
-      <c r="B38" s="248"/>
-      <c r="C38" s="248"/>
-      <c r="D38" s="248"/>
-      <c r="E38" s="248"/>
-      <c r="F38" s="248"/>
-      <c r="G38" s="248"/>
+      <c r="B38" s="250"/>
+      <c r="C38" s="250"/>
+      <c r="D38" s="250"/>
+      <c r="E38" s="250"/>
+      <c r="F38" s="250"/>
+      <c r="G38" s="250"/>
       <c r="H38" s="189"/>
       <c r="I38" s="189"/>
       <c r="J38" s="189"/>
@@ -15952,15 +15952,15 @@
       </c>
     </row>
     <row r="62" spans="1:10">
-      <c r="A62" s="246" t="s">
+      <c r="A62" s="249" t="s">
         <v>177</v>
       </c>
-      <c r="B62" s="246"/>
-      <c r="C62" s="246"/>
-      <c r="D62" s="246"/>
-      <c r="E62" s="246"/>
-      <c r="F62" s="246"/>
-      <c r="G62" s="246"/>
+      <c r="B62" s="249"/>
+      <c r="C62" s="249"/>
+      <c r="D62" s="249"/>
+      <c r="E62" s="249"/>
+      <c r="F62" s="249"/>
+      <c r="G62" s="249"/>
       <c r="H62" s="194"/>
       <c r="I62" s="194"/>
       <c r="J62" s="194"/>
@@ -15996,15 +15996,15 @@
       </c>
     </row>
     <row r="68" spans="1:10">
-      <c r="A68" s="245" t="s">
+      <c r="A68" s="248" t="s">
         <v>181</v>
       </c>
-      <c r="B68" s="245"/>
-      <c r="C68" s="245"/>
-      <c r="D68" s="245"/>
-      <c r="E68" s="245"/>
-      <c r="F68" s="245"/>
-      <c r="G68" s="245"/>
+      <c r="B68" s="248"/>
+      <c r="C68" s="248"/>
+      <c r="D68" s="248"/>
+      <c r="E68" s="248"/>
+      <c r="F68" s="248"/>
+      <c r="G68" s="248"/>
       <c r="H68" s="193"/>
       <c r="I68" s="193"/>
       <c r="J68" s="193"/>
@@ -16045,43 +16045,43 @@
       </c>
     </row>
     <row r="76" spans="1:10">
-      <c r="A76" s="247" t="s">
+      <c r="A76" s="246" t="s">
         <v>189</v>
       </c>
-      <c r="B76" s="244"/>
-      <c r="C76" s="244"/>
-      <c r="D76" s="244"/>
-      <c r="E76" s="244"/>
-      <c r="F76" s="244"/>
-      <c r="G76" s="244"/>
+      <c r="B76" s="245"/>
+      <c r="C76" s="245"/>
+      <c r="D76" s="245"/>
+      <c r="E76" s="245"/>
+      <c r="F76" s="245"/>
+      <c r="G76" s="245"/>
       <c r="H76" s="191"/>
       <c r="I76" s="191"/>
       <c r="J76" s="191"/>
     </row>
     <row r="77" spans="1:10">
-      <c r="A77" s="249" t="s">
+      <c r="A77" s="244" t="s">
         <v>190</v>
       </c>
-      <c r="B77" s="250"/>
-      <c r="C77" s="250"/>
-      <c r="D77" s="250"/>
-      <c r="E77" s="250"/>
-      <c r="F77" s="250"/>
-      <c r="G77" s="250"/>
+      <c r="B77" s="247"/>
+      <c r="C77" s="247"/>
+      <c r="D77" s="247"/>
+      <c r="E77" s="247"/>
+      <c r="F77" s="247"/>
+      <c r="G77" s="247"/>
       <c r="H77" s="192"/>
       <c r="I77" s="192"/>
       <c r="J77" s="192"/>
     </row>
     <row r="78" spans="1:10">
-      <c r="A78" s="244" t="s">
+      <c r="A78" s="245" t="s">
         <v>191</v>
       </c>
-      <c r="B78" s="244"/>
-      <c r="C78" s="244"/>
-      <c r="D78" s="244"/>
-      <c r="E78" s="244"/>
-      <c r="F78" s="244"/>
-      <c r="G78" s="244"/>
+      <c r="B78" s="245"/>
+      <c r="C78" s="245"/>
+      <c r="D78" s="245"/>
+      <c r="E78" s="245"/>
+      <c r="F78" s="245"/>
+      <c r="G78" s="245"/>
       <c r="H78" s="191"/>
       <c r="I78" s="191"/>
       <c r="J78" s="191"/>
@@ -16120,6 +16120,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A33:G33"/>
     <mergeCell ref="L1:R1"/>
     <mergeCell ref="A76:G76"/>
     <mergeCell ref="A77:G77"/>
@@ -16136,16 +16137,15 @@
     <mergeCell ref="A30:G30"/>
     <mergeCell ref="A31:G31"/>
     <mergeCell ref="A32:G32"/>
-    <mergeCell ref="A33:G33"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A70" r:id="rId1" location="SECTION004000000000000000000"/>
-    <hyperlink ref="A72" r:id="rId2"/>
-    <hyperlink ref="A77" r:id="rId3"/>
-    <hyperlink ref="A80" r:id="rId4"/>
-    <hyperlink ref="L1" r:id="rId5"/>
-    <hyperlink ref="E18" r:id="rId6"/>
-    <hyperlink ref="E19" r:id="rId7"/>
+    <hyperlink ref="A70" r:id="rId1" location="SECTION004000000000000000000" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="A72" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="A77" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="A80" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="L1" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="E18" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="E19" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId8"/>
@@ -16154,7 +16154,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O108"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -16968,15 +16968,15 @@
       <c r="O26" s="37"/>
     </row>
     <row r="27" spans="1:15" ht="38.25" customHeight="1">
-      <c r="A27" s="225" t="s">
+      <c r="A27" s="239" t="s">
         <v>262</v>
       </c>
-      <c r="B27" s="223"/>
-      <c r="C27" s="223"/>
-      <c r="D27" s="223"/>
-      <c r="E27" s="223"/>
-      <c r="F27" s="223"/>
-      <c r="G27" s="224"/>
+      <c r="B27" s="235"/>
+      <c r="C27" s="235"/>
+      <c r="D27" s="235"/>
+      <c r="E27" s="235"/>
+      <c r="F27" s="235"/>
+      <c r="G27" s="238"/>
       <c r="H27" s="195"/>
       <c r="I27" s="195"/>
       <c r="J27" s="195"/>
@@ -16987,15 +16987,15 @@
       <c r="O27" s="37"/>
     </row>
     <row r="28" spans="1:15" ht="63.75" customHeight="1">
-      <c r="A28" s="225" t="s">
+      <c r="A28" s="239" t="s">
         <v>263</v>
       </c>
-      <c r="B28" s="223"/>
-      <c r="C28" s="223"/>
-      <c r="D28" s="223"/>
-      <c r="E28" s="223"/>
-      <c r="F28" s="223"/>
-      <c r="G28" s="224"/>
+      <c r="B28" s="235"/>
+      <c r="C28" s="235"/>
+      <c r="D28" s="235"/>
+      <c r="E28" s="235"/>
+      <c r="F28" s="235"/>
+      <c r="G28" s="238"/>
       <c r="H28" s="195"/>
       <c r="I28" s="195"/>
       <c r="J28" s="195"/>
@@ -17006,15 +17006,15 @@
       <c r="O28" s="37"/>
     </row>
     <row r="29" spans="1:15" ht="51" customHeight="1">
-      <c r="A29" s="225" t="s">
+      <c r="A29" s="239" t="s">
         <v>264</v>
       </c>
-      <c r="B29" s="223"/>
-      <c r="C29" s="223"/>
-      <c r="D29" s="223"/>
-      <c r="E29" s="223"/>
-      <c r="F29" s="223"/>
-      <c r="G29" s="224"/>
+      <c r="B29" s="235"/>
+      <c r="C29" s="235"/>
+      <c r="D29" s="235"/>
+      <c r="E29" s="235"/>
+      <c r="F29" s="235"/>
+      <c r="G29" s="238"/>
       <c r="H29" s="195"/>
       <c r="I29" s="195"/>
       <c r="J29" s="195"/>
@@ -17025,15 +17025,15 @@
       <c r="O29" s="37"/>
     </row>
     <row r="30" spans="1:15" ht="51" customHeight="1">
-      <c r="A30" s="225" t="s">
+      <c r="A30" s="239" t="s">
         <v>265</v>
       </c>
-      <c r="B30" s="223"/>
-      <c r="C30" s="223"/>
-      <c r="D30" s="223"/>
-      <c r="E30" s="223"/>
-      <c r="F30" s="223"/>
-      <c r="G30" s="224"/>
+      <c r="B30" s="235"/>
+      <c r="C30" s="235"/>
+      <c r="D30" s="235"/>
+      <c r="E30" s="235"/>
+      <c r="F30" s="235"/>
+      <c r="G30" s="238"/>
       <c r="H30" s="195"/>
       <c r="I30" s="195"/>
       <c r="J30" s="195"/>
@@ -17044,15 +17044,15 @@
       <c r="O30" s="37"/>
     </row>
     <row r="31" spans="1:15">
-      <c r="A31" s="225" t="s">
+      <c r="A31" s="239" t="s">
         <v>266</v>
       </c>
-      <c r="B31" s="223"/>
-      <c r="C31" s="223"/>
-      <c r="D31" s="223"/>
-      <c r="E31" s="223"/>
-      <c r="F31" s="223"/>
-      <c r="G31" s="224"/>
+      <c r="B31" s="235"/>
+      <c r="C31" s="235"/>
+      <c r="D31" s="235"/>
+      <c r="E31" s="235"/>
+      <c r="F31" s="235"/>
+      <c r="G31" s="238"/>
       <c r="H31" s="195"/>
       <c r="I31" s="195"/>
       <c r="J31" s="195"/>
@@ -17225,10 +17225,10 @@
     <row r="40" spans="1:15">
       <c r="A40" s="183"/>
       <c r="B40" s="186"/>
-      <c r="C40" s="253" t="s">
+      <c r="C40" s="257" t="s">
         <v>272</v>
       </c>
-      <c r="D40" s="254" t="s">
+      <c r="D40" s="258" t="s">
         <v>273</v>
       </c>
       <c r="E40" s="198" t="s">
@@ -17250,8 +17250,8 @@
     <row r="41" spans="1:15">
       <c r="A41" s="183"/>
       <c r="B41" s="186"/>
-      <c r="C41" s="253"/>
-      <c r="D41" s="254"/>
+      <c r="C41" s="257"/>
+      <c r="D41" s="258"/>
       <c r="E41" s="198" t="s">
         <v>164</v>
       </c>
@@ -17352,19 +17352,19 @@
     <row r="45" spans="1:15">
       <c r="A45" s="183"/>
       <c r="B45" s="186"/>
-      <c r="C45" s="255" t="s">
+      <c r="C45" s="259" t="s">
         <v>288</v>
       </c>
       <c r="D45" s="13" t="s">
         <v>289</v>
       </c>
-      <c r="E45" s="256" t="s">
+      <c r="E45" s="260" t="s">
         <v>283</v>
       </c>
-      <c r="F45" s="259" t="s">
+      <c r="F45" s="255" t="s">
         <v>279</v>
       </c>
-      <c r="G45" s="257" t="s">
+      <c r="G45" s="252" t="s">
         <v>281</v>
       </c>
       <c r="H45" s="196"/>
@@ -17372,26 +17372,26 @@
       <c r="J45" s="196"/>
       <c r="K45" s="196"/>
       <c r="L45" s="170"/>
-      <c r="M45" s="257" t="s">
+      <c r="M45" s="252" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="46" spans="1:15" ht="15.75">
       <c r="A46" s="183"/>
       <c r="B46" s="186"/>
-      <c r="C46" s="255"/>
+      <c r="C46" s="259"/>
       <c r="D46" s="13" t="s">
         <v>290</v>
       </c>
-      <c r="E46" s="256"/>
-      <c r="F46" s="259"/>
-      <c r="G46" s="257"/>
+      <c r="E46" s="260"/>
+      <c r="F46" s="255"/>
+      <c r="G46" s="252"/>
       <c r="H46" s="196"/>
       <c r="I46" s="196"/>
       <c r="J46" s="196"/>
       <c r="K46" s="196"/>
       <c r="L46" s="170"/>
-      <c r="M46" s="257"/>
+      <c r="M46" s="252"/>
     </row>
     <row r="47" spans="1:15">
       <c r="A47" s="183"/>
@@ -17421,34 +17421,34 @@
       </c>
     </row>
     <row r="49" spans="3:13">
-      <c r="C49" s="243" t="s">
+      <c r="C49" s="221" t="s">
         <v>293</v>
       </c>
-      <c r="D49" s="243"/>
-      <c r="E49" s="243"/>
-      <c r="F49" s="243"/>
-      <c r="G49" s="243"/>
-      <c r="H49" s="243"/>
-      <c r="I49" s="243"/>
-      <c r="J49" s="243"/>
-      <c r="K49" s="243"/>
-      <c r="L49" s="243"/>
-      <c r="M49" s="243"/>
+      <c r="D49" s="221"/>
+      <c r="E49" s="221"/>
+      <c r="F49" s="221"/>
+      <c r="G49" s="221"/>
+      <c r="H49" s="221"/>
+      <c r="I49" s="221"/>
+      <c r="J49" s="221"/>
+      <c r="K49" s="221"/>
+      <c r="L49" s="221"/>
+      <c r="M49" s="221"/>
     </row>
     <row r="50" spans="3:13">
-      <c r="C50" s="239" t="s">
+      <c r="C50" s="222" t="s">
         <v>294</v>
       </c>
-      <c r="D50" s="239"/>
-      <c r="E50" s="239"/>
-      <c r="F50" s="239"/>
-      <c r="G50" s="239"/>
-      <c r="H50" s="239"/>
-      <c r="I50" s="239"/>
-      <c r="J50" s="239"/>
-      <c r="K50" s="239"/>
-      <c r="L50" s="239"/>
-      <c r="M50" s="239"/>
+      <c r="D50" s="222"/>
+      <c r="E50" s="222"/>
+      <c r="F50" s="222"/>
+      <c r="G50" s="222"/>
+      <c r="H50" s="222"/>
+      <c r="I50" s="222"/>
+      <c r="J50" s="222"/>
+      <c r="K50" s="222"/>
+      <c r="L50" s="222"/>
+      <c r="M50" s="222"/>
     </row>
     <row r="51" spans="3:13">
       <c r="C51" s="17"/>
@@ -17909,13 +17909,13 @@
       <c r="L72" s="172"/>
     </row>
     <row r="73" spans="3:12">
-      <c r="C73" s="251" t="s">
+      <c r="C73" s="253" t="s">
         <v>316</v>
       </c>
-      <c r="D73" s="251" t="s">
+      <c r="D73" s="253" t="s">
         <v>319</v>
       </c>
-      <c r="E73" s="251" t="s">
+      <c r="E73" s="253" t="s">
         <v>319</v>
       </c>
       <c r="F73" s="19" t="s">
@@ -17931,9 +17931,9 @@
       <c r="L73" s="173"/>
     </row>
     <row r="74" spans="3:12">
-      <c r="C74" s="258"/>
-      <c r="D74" s="258"/>
-      <c r="E74" s="258"/>
+      <c r="C74" s="254"/>
+      <c r="D74" s="254"/>
+      <c r="E74" s="254"/>
       <c r="F74" s="20" t="s">
         <v>340</v>
       </c>
@@ -17947,9 +17947,9 @@
       <c r="L74" s="173"/>
     </row>
     <row r="75" spans="3:12">
-      <c r="C75" s="258"/>
-      <c r="D75" s="258"/>
-      <c r="E75" s="258"/>
+      <c r="C75" s="254"/>
+      <c r="D75" s="254"/>
+      <c r="E75" s="254"/>
       <c r="F75" s="20" t="s">
         <v>342</v>
       </c>
@@ -17963,9 +17963,9 @@
       <c r="L75" s="173"/>
     </row>
     <row r="76" spans="3:12">
-      <c r="C76" s="258"/>
-      <c r="D76" s="258"/>
-      <c r="E76" s="258"/>
+      <c r="C76" s="254"/>
+      <c r="D76" s="254"/>
+      <c r="E76" s="254"/>
       <c r="F76" s="20" t="s">
         <v>344</v>
       </c>
@@ -17979,13 +17979,13 @@
       <c r="L76" s="173"/>
     </row>
     <row r="77" spans="3:12">
-      <c r="C77" s="251" t="s">
+      <c r="C77" s="253" t="s">
         <v>321</v>
       </c>
-      <c r="D77" s="251" t="s">
+      <c r="D77" s="253" t="s">
         <v>319</v>
       </c>
-      <c r="E77" s="251" t="s">
+      <c r="E77" s="253" t="s">
         <v>319</v>
       </c>
       <c r="F77" s="19" t="s">
@@ -18001,9 +18001,9 @@
       <c r="L77" s="173"/>
     </row>
     <row r="78" spans="3:12">
-      <c r="C78" s="252"/>
-      <c r="D78" s="252"/>
-      <c r="E78" s="252"/>
+      <c r="C78" s="256"/>
+      <c r="D78" s="256"/>
+      <c r="E78" s="256"/>
       <c r="F78" s="21" t="s">
         <v>348</v>
       </c>
@@ -18257,13 +18257,13 @@
       <c r="L90" s="172"/>
     </row>
     <row r="92" spans="3:12">
-      <c r="C92" s="221" t="s">
+      <c r="C92" s="236" t="s">
         <v>367</v>
       </c>
-      <c r="D92" s="221"/>
-      <c r="E92" s="221"/>
-      <c r="F92" s="221"/>
-      <c r="G92" s="221"/>
+      <c r="D92" s="236"/>
+      <c r="E92" s="236"/>
+      <c r="F92" s="236"/>
+      <c r="G92" s="236"/>
       <c r="H92" s="186"/>
       <c r="I92" s="186"/>
       <c r="J92" s="186"/>
@@ -18271,13 +18271,13 @@
       <c r="L92" s="183"/>
     </row>
     <row r="93" spans="3:12">
-      <c r="C93" s="221" t="s">
+      <c r="C93" s="236" t="s">
         <v>368</v>
       </c>
-      <c r="D93" s="221"/>
-      <c r="E93" s="221"/>
-      <c r="F93" s="221"/>
-      <c r="G93" s="221"/>
+      <c r="D93" s="236"/>
+      <c r="E93" s="236"/>
+      <c r="F93" s="236"/>
+      <c r="G93" s="236"/>
       <c r="H93" s="186"/>
       <c r="I93" s="186"/>
       <c r="J93" s="186"/>
@@ -18389,24 +18389,24 @@
       <c r="I101" s="183"/>
     </row>
     <row r="103" spans="3:9">
-      <c r="C103" s="260" t="s">
+      <c r="C103" s="251" t="s">
         <v>374</v>
       </c>
-      <c r="D103" s="260" t="s">
+      <c r="D103" s="251" t="s">
         <v>380</v>
       </c>
-      <c r="E103" s="260"/>
-      <c r="F103" s="260" t="s">
+      <c r="E103" s="251"/>
+      <c r="F103" s="251" t="s">
         <v>381</v>
       </c>
-      <c r="G103" s="260"/>
-      <c r="H103" s="260" t="s">
+      <c r="G103" s="251"/>
+      <c r="H103" s="251" t="s">
         <v>375</v>
       </c>
-      <c r="I103" s="260"/>
+      <c r="I103" s="251"/>
     </row>
     <row r="104" spans="3:9">
-      <c r="C104" s="260"/>
+      <c r="C104" s="251"/>
       <c r="D104" s="195" t="s">
         <v>382</v>
       </c>
@@ -18508,20 +18508,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="C103:C104"/>
-    <mergeCell ref="D103:E103"/>
-    <mergeCell ref="F103:G103"/>
-    <mergeCell ref="H103:I103"/>
-    <mergeCell ref="C92:G92"/>
-    <mergeCell ref="C93:G93"/>
-    <mergeCell ref="M45:M46"/>
-    <mergeCell ref="C49:M49"/>
-    <mergeCell ref="C50:M50"/>
-    <mergeCell ref="G45:G46"/>
-    <mergeCell ref="C73:C76"/>
-    <mergeCell ref="D73:D76"/>
-    <mergeCell ref="E73:E76"/>
-    <mergeCell ref="F45:F46"/>
     <mergeCell ref="A27:G27"/>
     <mergeCell ref="A28:G28"/>
     <mergeCell ref="C77:C78"/>
@@ -18534,18 +18520,32 @@
     <mergeCell ref="A30:G30"/>
     <mergeCell ref="A29:G29"/>
     <mergeCell ref="A31:G31"/>
+    <mergeCell ref="M45:M46"/>
+    <mergeCell ref="C49:M49"/>
+    <mergeCell ref="C50:M50"/>
+    <mergeCell ref="G45:G46"/>
+    <mergeCell ref="C73:C76"/>
+    <mergeCell ref="D73:D76"/>
+    <mergeCell ref="E73:E76"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="C103:C104"/>
+    <mergeCell ref="D103:E103"/>
+    <mergeCell ref="F103:G103"/>
+    <mergeCell ref="H103:I103"/>
+    <mergeCell ref="C92:G92"/>
+    <mergeCell ref="C93:G93"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D40" r:id="rId1" tooltip="Array data structure" display="http://en.wikipedia.org/wiki/Array_data_structure"/>
-    <hyperlink ref="E40" r:id="rId2" tooltip="Dynamic array" display="http://en.wikipedia.org/wiki/Dynamic_array"/>
-    <hyperlink ref="E41" r:id="rId3" tooltip="Dynamic array" display="http://en.wikipedia.org/wiki/Dynamic_array"/>
-    <hyperlink ref="F40" r:id="rId4" tooltip="Self-balancing binary search tree" display="http://en.wikipedia.org/wiki/Self-balancing_binary_search_tree"/>
-    <hyperlink ref="F41" r:id="rId5" tooltip="Self-balancing binary search tree" display="http://en.wikipedia.org/wiki/Self-balancing_binary_search_tree"/>
-    <hyperlink ref="G40" r:id="rId6" tooltip="Random access list (page does not exist)" display="http://en.wikipedia.org/w/index.php?title=Random_access_list&amp;action=edit&amp;redlink=1"/>
-    <hyperlink ref="G41" r:id="rId7" tooltip="Random access list (page does not exist)" display="http://en.wikipedia.org/w/index.php?title=Random_access_list&amp;action=edit&amp;redlink=1"/>
-    <hyperlink ref="F44" r:id="rId8" tooltip="Amortized analysis" display="http://en.wikipedia.org/wiki/Amortized_analysis"/>
-    <hyperlink ref="F47" r:id="rId9" location="cite_note-brodnik-4" display="http://en.wikipedia.org/wiki/Linked_list - cite_note-brodnik-4"/>
-    <hyperlink ref="O2" r:id="rId10"/>
+    <hyperlink ref="D40" r:id="rId1" tooltip="Array data structure" display="http://en.wikipedia.org/wiki/Array_data_structure" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="E40" r:id="rId2" tooltip="Dynamic array" display="http://en.wikipedia.org/wiki/Dynamic_array" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="E41" r:id="rId3" tooltip="Dynamic array" display="http://en.wikipedia.org/wiki/Dynamic_array" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="F40" r:id="rId4" tooltip="Self-balancing binary search tree" display="http://en.wikipedia.org/wiki/Self-balancing_binary_search_tree" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="F41" r:id="rId5" tooltip="Self-balancing binary search tree" display="http://en.wikipedia.org/wiki/Self-balancing_binary_search_tree" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="G40" r:id="rId6" tooltip="Random access list (page does not exist)" display="http://en.wikipedia.org/w/index.php?title=Random_access_list&amp;action=edit&amp;redlink=1" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="G41" r:id="rId7" tooltip="Random access list (page does not exist)" display="http://en.wikipedia.org/w/index.php?title=Random_access_list&amp;action=edit&amp;redlink=1" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
+    <hyperlink ref="F44" r:id="rId8" tooltip="Amortized analysis" display="http://en.wikipedia.org/wiki/Amortized_analysis" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
+    <hyperlink ref="F47" r:id="rId9" location="cite_note-brodnik-4" display="http://en.wikipedia.org/wiki/Linked_list - cite_note-brodnik-4" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
+    <hyperlink ref="O2" r:id="rId10" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId11"/>
@@ -18553,7 +18553,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18655,7 +18655,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AO62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -20103,13 +20103,13 @@
       </c>
     </row>
     <row r="62" spans="3:9" ht="71.25" customHeight="1">
-      <c r="C62" s="221" t="s">
+      <c r="C62" s="236" t="s">
         <v>549</v>
       </c>
-      <c r="D62" s="221"/>
-      <c r="E62" s="221"/>
-      <c r="F62" s="221"/>
-      <c r="G62" s="221"/>
+      <c r="D62" s="236"/>
+      <c r="E62" s="236"/>
+      <c r="F62" s="236"/>
+      <c r="G62" s="236"/>
       <c r="H62" s="186"/>
       <c r="I62" s="186"/>
     </row>
@@ -20119,7 +20119,7 @@
     <mergeCell ref="E1:G1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C44" r:id="rId1"/>
+    <hyperlink ref="C44" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -20127,7 +20127,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -20817,7 +20817,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:BM86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -23585,15 +23585,15 @@
     <mergeCell ref="A76:G76"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A83" r:id="rId1"/>
-    <hyperlink ref="H35" r:id="rId2"/>
-    <hyperlink ref="H43" r:id="rId3"/>
-    <hyperlink ref="H44" r:id="rId4"/>
-    <hyperlink ref="H49" r:id="rId5"/>
-    <hyperlink ref="H52" r:id="rId6"/>
-    <hyperlink ref="H50" r:id="rId7"/>
-    <hyperlink ref="H36" r:id="rId8"/>
-    <hyperlink ref="G54" r:id="rId9"/>
+    <hyperlink ref="A83" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="H35" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
+    <hyperlink ref="H43" r:id="rId3" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
+    <hyperlink ref="H44" r:id="rId4" xr:uid="{00000000-0004-0000-0600-000003000000}"/>
+    <hyperlink ref="H49" r:id="rId5" xr:uid="{00000000-0004-0000-0600-000004000000}"/>
+    <hyperlink ref="H52" r:id="rId6" xr:uid="{00000000-0004-0000-0600-000005000000}"/>
+    <hyperlink ref="H50" r:id="rId7" xr:uid="{00000000-0004-0000-0600-000006000000}"/>
+    <hyperlink ref="H36" r:id="rId8" xr:uid="{00000000-0004-0000-0600-000007000000}"/>
+    <hyperlink ref="G54" r:id="rId9" xr:uid="{00000000-0004-0000-0600-000008000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId10"/>
@@ -23601,7 +23601,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -23715,10 +23715,10 @@
     <mergeCell ref="B11:B12"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1"/>
-    <hyperlink ref="C7" r:id="rId2"/>
-    <hyperlink ref="B13" r:id="rId3"/>
-    <hyperlink ref="B1" r:id="rId4" display="http://msdn.microsoft.com/en-us/library/vstudio/yht2cx7b(v=vs.100).aspx"/>
+    <hyperlink ref="C4" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
+    <hyperlink ref="C7" r:id="rId2" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
+    <hyperlink ref="B13" r:id="rId3" xr:uid="{00000000-0004-0000-0700-000002000000}"/>
+    <hyperlink ref="B1" r:id="rId4" display="http://msdn.microsoft.com/en-us/library/vstudio/yht2cx7b(v=vs.100).aspx" xr:uid="{00000000-0004-0000-0700-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
@@ -23726,7 +23726,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:T37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -24940,17 +24940,17 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F27" r:id="rId1"/>
-    <hyperlink ref="G27" r:id="rId2" display="http://msdn.microsoft.com/en-us/library/bb359438(v=vs.110).aspx"/>
-    <hyperlink ref="B27" r:id="rId3" display="http://msdn.microsoft.com/en-us/library/aa288453(v=vs.71).aspx "/>
-    <hyperlink ref="M27" r:id="rId4"/>
-    <hyperlink ref="O27" r:id="rId5"/>
-    <hyperlink ref="Q27" r:id="rId6"/>
-    <hyperlink ref="S27" r:id="rId7"/>
-    <hyperlink ref="T27" r:id="rId8" display="http://blogs.msdn.com/b/bclteam/archive/2012/12/18/preview-of-immutable-collections-released-on-nuget.aspx"/>
-    <hyperlink ref="I27" r:id="rId9"/>
-    <hyperlink ref="C27" r:id="rId10"/>
-    <hyperlink ref="D27" r:id="rId11"/>
+    <hyperlink ref="F27" r:id="rId1" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
+    <hyperlink ref="G27" r:id="rId2" display="http://msdn.microsoft.com/en-us/library/bb359438(v=vs.110).aspx" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
+    <hyperlink ref="B27" r:id="rId3" display="http://msdn.microsoft.com/en-us/library/aa288453(v=vs.71).aspx " xr:uid="{00000000-0004-0000-0800-000002000000}"/>
+    <hyperlink ref="M27" r:id="rId4" xr:uid="{00000000-0004-0000-0800-000003000000}"/>
+    <hyperlink ref="O27" r:id="rId5" xr:uid="{00000000-0004-0000-0800-000004000000}"/>
+    <hyperlink ref="Q27" r:id="rId6" xr:uid="{00000000-0004-0000-0800-000005000000}"/>
+    <hyperlink ref="S27" r:id="rId7" xr:uid="{00000000-0004-0000-0800-000006000000}"/>
+    <hyperlink ref="T27" r:id="rId8" display="http://blogs.msdn.com/b/bclteam/archive/2012/12/18/preview-of-immutable-collections-released-on-nuget.aspx" xr:uid="{00000000-0004-0000-0800-000007000000}"/>
+    <hyperlink ref="I27" r:id="rId9" xr:uid="{00000000-0004-0000-0800-000008000000}"/>
+    <hyperlink ref="C27" r:id="rId10" xr:uid="{00000000-0004-0000-0800-000009000000}"/>
+    <hyperlink ref="D27" r:id="rId11" xr:uid="{00000000-0004-0000-0800-00000A000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId12"/>

</xml_diff>